<commit_message>
chore: update dependencies and improve styling in AchievementListScreen
- Updated expo and expo-font versions in package.json for better compatibility.
- Changed background color in AchievementListScreen from transparent to white for improved visibility.
- Cleaned up code formatting in AchievementListScreen.
</commit_message>
<xml_diff>
--- a/docs/テスト仕様書_20251124.xlsx
+++ b/docs/テスト仕様書_20251124.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janne\source\little-baby-age-expo54\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D563C43-AFAA-40AD-A2B0-C65847A2ED48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97842E65-7ED5-40DB-BD78-7DFDAAAF12AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A7B97F13-BAE2-4B77-8BB6-3D1A54252199}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A7B97F13-BAE2-4B77-8BB6-3D1A54252199}"/>
   </bookViews>
   <sheets>
     <sheet name="テスト仕様書" sheetId="1" r:id="rId1"/>
     <sheet name="iosテスト" sheetId="2" r:id="rId2"/>
-    <sheet name="ブラウザ版でのテスト" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="418">
   <si>
     <t>項目ID</t>
   </si>
@@ -1040,10 +1039,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>×</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>判定</t>
     <rPh sb="0" eb="2">
       <t>ハンテイ</t>
@@ -1052,10 +1047,6 @@
   </si>
   <si>
     <t>出生日=2025-01-10, 出産予定日=未入力</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>OK</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
@@ -1459,510 +1450,9 @@
     <t>何か詰まったら教えてください。</t>
   </si>
   <si>
-    <t>結論を先にまとめると：</t>
-  </si>
-  <si>
-    <t>✅ Expo（Web＝“w”）で起動した場合、保存データは「ブラウザの開発者ツール」で確認できます。</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Expo Web 版は </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>AsyncStorage → LocalStorage にマッピング</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>されます。</t>
-    </r>
-  </si>
-  <si>
-    <t>つまり Web で動いているときは、</t>
-  </si>
-  <si>
-    <t>React Native の AsyncStorage ではなく</t>
-  </si>
-  <si>
-    <t>ブラウザの LocalStorage に保存される</t>
-  </si>
-  <si>
-    <t>という挙動になります。</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">そのため、保存データを確認する方法は </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>ブラウザの開発者ツール（DevTools）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve"> を使うのが最も簡単です。</t>
-    </r>
-  </si>
-  <si>
-    <t>🔍 手順：Expo Web で保存データを確認する方法（Chromeの場合）</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>npx expo start</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13.5"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve"> を実行</t>
-    </r>
-  </si>
-  <si>
-    <t>2. 「w」キーを押して Web で起動</t>
-  </si>
-  <si>
-    <t>→ Chrome（またはデフォルトブラウザ）でアプリが開く</t>
-  </si>
-  <si>
-    <t>3. ブラウザで F12 か 右クリック → 検証</t>
-  </si>
-  <si>
-    <t>→ DevTools が開く</t>
-  </si>
-  <si>
-    <t>4. 上部タブから Application を選択</t>
-  </si>
-  <si>
-    <t>→ 左側の Navigation にストレージ一覧がある</t>
-  </si>
-  <si>
-    <t>5. 左メニューの Local Storage → https://localhost:19006 を選択</t>
-  </si>
-  <si>
-    <t>（URLは環境で異なる）</t>
-  </si>
-  <si>
-    <t>6. ここに下記のキーが保存されています</t>
-  </si>
-  <si>
-    <t>little_baby_calendar_user_settings    {"birthDate":"2025-01-10","dueDate":"2025-03-01","ageFormat":"md", ...}</t>
-  </si>
-  <si>
-    <t>little_baby_calendar_achievements     {"achievements":[{"id":"uuid","title":"..."}, ... ]}</t>
-  </si>
-  <si>
-    <t>クリックすると JSON をそのまま確認できます。</t>
-  </si>
-  <si>
-    <t>🟦 注意：Expo Web の保存は “端末側（AsyncStorage）とは別物”</t>
-  </si>
-  <si>
-    <t>Expo Web は「ブラウザ」で動いているため、</t>
-  </si>
-  <si>
-    <r>
-      <t>同じアプリでも Expo Go（実機）とは別の保存領域</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>です。</t>
-    </r>
-  </si>
-  <si>
-    <t>つまり：</t>
-  </si>
-  <si>
-    <t>Expo Web の LocalStorage</t>
-  </si>
-  <si>
-    <t>→ ブラウザごとに保存（Chromeだけ、Safariだけ）</t>
-  </si>
-  <si>
-    <t>iPhone / Android の AsyncStorage</t>
-  </si>
-  <si>
-    <t>→ アプリ側に保存（React Native Debuggerで見えるやつ）</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">これらは </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>同期しません</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>。</t>
-    </r>
-  </si>
-  <si>
-    <t>（テスト目的なら問題なし）</t>
-  </si>
-  <si>
-    <t>🎯 まとめ（あなたの質問への回答）</t>
-  </si>
-  <si>
-    <t>「w」でブラウザから確認できるとき、保存データはどうやったら見れる？</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">👉 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>ブラウザ開発者ツール → Application → LocalStorage</t>
-    </r>
-  </si>
-  <si>
-    <t>に保存されている値が、あなたのアプリの保存データです。</t>
-  </si>
-  <si>
-    <t>コード変更はゼロで確認できます。</t>
-  </si>
-  <si>
-    <t>必要なら案内できます</t>
-  </si>
-  <si>
-    <t>LocalStorage の中身を JSON として整形して見やすくする方法</t>
-  </si>
-  <si>
-    <t>LocalStorage を手動で削除して初期化する方法</t>
-  </si>
-  <si>
-    <t>Web版でのデータ破損の直し方</t>
-  </si>
-  <si>
-    <t>本番ビルドした Web 版でも同じように確認できるか（→できます）</t>
-  </si>
-  <si>
-    <t>どれを知りたいですか？</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Expo Web（“w”）で動かしている場合、保存データ（AsyncStorage → LocalStorageへのマッピング）は </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>ブラウザの LocalStorage を削除することで初期化できます</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>。</t>
-    </r>
-  </si>
-  <si>
-    <t>とても簡単です。以下の手順で “完全初期化” できます。</t>
-  </si>
-  <si>
-    <t>✅ LocalStorage を手動で削除して初期化する方法（Chrome）</t>
-  </si>
-  <si>
-    <t>① ブラウザでアプリを表示</t>
-  </si>
-  <si>
-    <r>
-      <t>npx expo start → w</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve"> でアプリが開いた状態にする。</t>
-    </r>
-  </si>
-  <si>
-    <t>② F12 または 右クリック「検証」で DevTools を開く</t>
-  </si>
-  <si>
-    <t>③ タブ Application を選ぶ</t>
-  </si>
-  <si>
-    <t>上部の以下の場所にあります：</t>
-  </si>
-  <si>
-    <t>Elements  Console  Sources  Network  ...  Application</t>
-  </si>
-  <si>
-    <t>④ 左のメニュー → Local Storage → 自分の URL を選択</t>
-  </si>
-  <si>
-    <t>例）</t>
-  </si>
-  <si>
-    <t>Local Storage</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> └ https://localhost:19006</t>
-  </si>
-  <si>
-    <t>⑤ 保存されているキー一覧が表示される</t>
-  </si>
-  <si>
-    <t>あなたのアプリの場合：</t>
-  </si>
-  <si>
-    <t>などが表示されます。</t>
-  </si>
-  <si>
-    <t>⑥ 削除する方法（どれでもOK）</t>
-  </si>
-  <si>
-    <t>方法 A）キーを個別に削除</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">各キーを右クリック → </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>Delete</t>
-    </r>
-  </si>
-  <si>
-    <t>方法 B）すべて消す（推奨）</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Local Storage 項目を右クリック → </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>Clear</t>
-    </r>
-  </si>
-  <si>
-    <t>方法 C）上部にある「×（Clear All）」を押す</t>
-  </si>
-  <si>
-    <t>これでも全部消える。</t>
-  </si>
-  <si>
-    <t>🧹 削除後にどうなる？</t>
-  </si>
-  <si>
-    <t>ブラウザをリロードすると：</t>
-  </si>
-  <si>
-    <t>初回起動時と同じ状態になる</t>
-  </si>
-  <si>
-    <t>S-01（初回セットアップ画面）が出る</t>
-  </si>
-  <si>
-    <t>Achievements も全消去される</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">つまり </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>完全に初期化された状態</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve"> です。</t>
-    </r>
-  </si>
-  <si>
-    <t>🔍 補足：Safari / Edge の場合もほぼ同じ</t>
-  </si>
-  <si>
-    <t>Safari：</t>
-  </si>
-  <si>
-    <t>→ 「Develop → Web Inspector → Storage → LocalStorage」</t>
-  </si>
-  <si>
-    <t>Edge：</t>
-  </si>
-  <si>
-    <t>→ Chrome とほぼ同じ UI</t>
-  </si>
-  <si>
-    <t>🎯 最後に（あなたへの最適運用）</t>
-  </si>
-  <si>
-    <t>Web 版テストでは：</t>
-  </si>
-  <si>
-    <t>データを消したい時は LocalStorage を Clear</t>
-  </si>
-  <si>
-    <t>実機・Expo Go では React Native Debugger（Storage Inspector）を使う</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">これで </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>両方の環境でデータの確認・初期化が可能</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>になります。</t>
-    </r>
-  </si>
-  <si>
-    <t>必要なら：</t>
-  </si>
-  <si>
-    <t>初期化用の「ワンクリックリセットボタン」をつくらずに、</t>
-  </si>
-  <si>
-    <r>
-      <t>開発者だけ使える隠し操作</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Meiryo UI"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve"> の案も出します。</t>
-    </r>
-  </si>
-  <si>
-    <t>続けて何かありますか？</t>
-  </si>
-  <si>
     <t>詳細</t>
     <rPh sb="0" eb="2">
       <t>ショウサイ</t>
-    </rPh>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>「カレンダーへ」というボタン名である</t>
-    <rPh sb="14" eb="15">
-      <t>メイ</t>
     </rPh>
     <phoneticPr fontId="18"/>
   </si>
@@ -2000,9 +1490,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="184" formatCode="m/d;@"/>
+    <numFmt numFmtId="176" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -2180,21 +1670,6 @@
       <color theme="10"/>
       <name val="Meiryo UI"/>
       <family val="2"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Meiryo UI"/>
-      <family val="3"/>
       <charset val="128"/>
     </font>
   </fonts>
@@ -2673,7 +2148,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2728,26 +2203,17 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="42">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -3138,8 +2604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66320BD9-D84F-418E-93A3-BA2DA31DDDD4}">
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3151,7 +2617,7 @@
     <col min="5" max="6" width="32.453125" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.7265625" style="1" customWidth="1"/>
     <col min="8" max="8" width="4.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" style="20" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3178,16 +2644,16 @@
         <v>334</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="I1" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="I1" s="18" t="s">
         <v>335</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="57.6">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="28.8">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -3206,16 +2672,9 @@
       <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="24" t="s">
-        <v>502</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="I2" s="21">
-        <v>46001</v>
-      </c>
-      <c r="J2" s="24"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="28.8">
       <c r="A3" s="4" t="s">
@@ -3228,7 +2687,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>13</v>
@@ -3236,12 +2695,7 @@
       <c r="F3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="I3" s="22">
-        <v>46001</v>
-      </c>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="28.8">
       <c r="A4" s="4" t="s">
@@ -3254,7 +2708,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>503</v>
+        <v>414</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>13</v>
@@ -3262,162 +2716,147 @@
       <c r="F4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="I4" s="22">
-        <v>46001</v>
-      </c>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="28.8">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="26" t="s">
+      <c r="C5" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="I5" s="22">
-        <v>46001</v>
-      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="28.8">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="26" t="s">
+      <c r="C6" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="I6" s="22">
-        <v>46001</v>
-      </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="28.8">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="26" t="s">
+      <c r="C7" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="23" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="28.8">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="26" t="s">
+      <c r="C8" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="28.8">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="26" t="s">
+      <c r="C9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="23" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="28.8">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="23" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.8">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="26" t="s">
+      <c r="C11" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="23" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3440,12 +2879,7 @@
       <c r="F12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I12" s="22">
-        <v>46001</v>
-      </c>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="28.8">
       <c r="A13" s="4" t="s">
@@ -3466,12 +2900,7 @@
       <c r="F13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I13" s="22">
-        <v>46001</v>
-      </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="28.8">
       <c r="A14" s="4" t="s">
@@ -3492,70 +2921,65 @@
       <c r="F14" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I14" s="22">
-        <v>46001</v>
-      </c>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:10" ht="28.8">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="26" t="s">
+      <c r="D15" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="23" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="28.8">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="26" t="s">
+      <c r="D16" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="23" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="28.8">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="26" t="s">
+      <c r="D17" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="23" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3579,9 +3003,9 @@
         <v>71</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I18" s="22">
+        <v>415</v>
+      </c>
+      <c r="I18" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -3605,9 +3029,9 @@
         <v>74</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I19" s="22">
+        <v>415</v>
+      </c>
+      <c r="I19" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -3631,9 +3055,9 @@
         <v>78</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I20" s="22">
+        <v>415</v>
+      </c>
+      <c r="I20" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -3657,29 +3081,29 @@
         <v>82</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I21" s="22">
+        <v>415</v>
+      </c>
+      <c r="I21" s="20">
         <v>46001</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="28.8">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="26" t="s">
+      <c r="D22" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="F22" s="26" t="s">
+      <c r="F22" s="23" t="s">
         <v>86</v>
       </c>
     </row>
@@ -3703,9 +3127,9 @@
         <v>90</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I23" s="22">
+        <v>415</v>
+      </c>
+      <c r="I23" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -3729,9 +3153,9 @@
         <v>94</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I24" s="22">
+        <v>415</v>
+      </c>
+      <c r="I24" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -3755,9 +3179,9 @@
         <v>99</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I25" s="22">
+        <v>415</v>
+      </c>
+      <c r="I25" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -3781,9 +3205,9 @@
         <v>103</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I26" s="22">
+        <v>415</v>
+      </c>
+      <c r="I26" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -4084,10 +3508,10 @@
         <v>160</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>505</v>
+        <v>416</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>506</v>
+        <v>417</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="28.8">
@@ -4110,9 +3534,9 @@
         <v>165</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I42" s="22">
+        <v>415</v>
+      </c>
+      <c r="I42" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -4276,9 +3700,9 @@
         <v>195</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I50" s="22">
+        <v>415</v>
+      </c>
+      <c r="I50" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -4322,9 +3746,9 @@
         <v>203</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I52" s="22">
+        <v>415</v>
+      </c>
+      <c r="I52" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -4348,9 +3772,9 @@
         <v>207</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I53" s="22">
+        <v>415</v>
+      </c>
+      <c r="I53" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -4374,9 +3798,9 @@
         <v>212</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I54" s="22">
+        <v>415</v>
+      </c>
+      <c r="I54" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -4400,9 +3824,9 @@
         <v>217</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I55" s="22">
+        <v>415</v>
+      </c>
+      <c r="I55" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -4426,9 +3850,9 @@
         <v>222</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I56" s="22">
+        <v>415</v>
+      </c>
+      <c r="I56" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -4452,9 +3876,9 @@
         <v>226</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I57" s="22">
+        <v>415</v>
+      </c>
+      <c r="I57" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -4478,9 +3902,9 @@
         <v>230</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I58" s="22">
+        <v>415</v>
+      </c>
+      <c r="I58" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -4524,9 +3948,9 @@
         <v>238</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I60" s="22">
+        <v>415</v>
+      </c>
+      <c r="I60" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -4610,9 +4034,9 @@
         <v>255</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="I64" s="22">
+        <v>415</v>
+      </c>
+      <c r="I64" s="20">
         <v>46001</v>
       </c>
     </row>
@@ -4957,7 +4381,7 @@
       </c>
       <c r="G81" s="9"/>
       <c r="H81" s="7"/>
-      <c r="I81" s="23"/>
+      <c r="I81" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>
@@ -4977,37 +4401,37 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="10" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="31.8">
       <c r="A8" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="31.8">
       <c r="A14" s="11" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="15" spans="1:1">
@@ -5015,7 +4439,7 @@
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -5023,7 +4447,7 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="12" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="19" spans="1:1">
@@ -5031,17 +4455,17 @@
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="31.8">
       <c r="A24" s="11" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="18.600000000000001">
       <c r="A26" s="13" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="27" spans="1:1">
@@ -5049,12 +4473,12 @@
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="12" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="14" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="30" spans="1:1">
@@ -5062,7 +4486,7 @@
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="16" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="32" spans="1:1">
@@ -5070,17 +4494,17 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="12" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="16" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="18.600000000000001">
       <c r="A36" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="37" spans="1:1">
@@ -5088,47 +4512,47 @@
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="16" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="31.8">
       <c r="A42" s="11" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="15" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="15" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="31.8">
       <c r="A55" s="11" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="58" spans="1:1">
@@ -5136,7 +4560,7 @@
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="60" spans="1:1">
@@ -5144,47 +4568,47 @@
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="18.600000000000001">
       <c r="A63" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="31.8">
       <c r="A69" s="11" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="18.600000000000001">
       <c r="A73" s="13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="18.600000000000001">
       <c r="A79" s="13" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="80" spans="1:1">
@@ -5192,7 +4616,7 @@
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="16" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="82" spans="1:1">
@@ -5200,82 +4624,82 @@
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="16" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="18.600000000000001">
       <c r="A85" s="13" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="15" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="15" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="15" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="15" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="31.8">
       <c r="A98" s="11" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="18.600000000000001">
       <c r="A102" s="13" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="18.600000000000001">
       <c r="A104" s="13" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="31.8">
       <c r="A110" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="113" spans="1:1">
@@ -5283,7 +4707,7 @@
     </row>
     <row r="114" spans="1:1">
       <c r="A114" s="17" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="115" spans="1:1">
@@ -5291,7 +4715,7 @@
     </row>
     <row r="116" spans="1:1">
       <c r="A116" s="17" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="117" spans="1:1">
@@ -5299,7 +4723,7 @@
     </row>
     <row r="118" spans="1:1">
       <c r="A118" s="17" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="119" spans="1:1">
@@ -5307,17 +4731,17 @@
     </row>
     <row r="120" spans="1:1">
       <c r="A120" s="17" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="125" spans="1:1">
@@ -5325,7 +4749,7 @@
     </row>
     <row r="126" spans="1:1">
       <c r="A126" s="16" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="127" spans="1:1">
@@ -5333,7 +4757,7 @@
     </row>
     <row r="128" spans="1:1">
       <c r="A128" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="129" spans="1:1">
@@ -5341,17 +4765,17 @@
     </row>
     <row r="130" spans="1:1">
       <c r="A130" s="12" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="31.8">
       <c r="A134" s="11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="137" spans="1:1">
@@ -5359,22 +4783,22 @@
     </row>
     <row r="138" spans="1:1">
       <c r="A138" s="12" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" s="12" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="31.8">
       <c r="A145" s="11" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="146" spans="1:1">
@@ -5382,7 +4806,7 @@
     </row>
     <row r="147" spans="1:1">
       <c r="A147" s="12" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="148" spans="1:1">
@@ -5390,7 +4814,7 @@
     </row>
     <row r="149" spans="1:1">
       <c r="A149" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="150" spans="1:1">
@@ -5398,7 +4822,7 @@
     </row>
     <row r="151" spans="1:1">
       <c r="A151" s="12" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="152" spans="1:1">
@@ -5406,7 +4830,7 @@
     </row>
     <row r="153" spans="1:1">
       <c r="A153" s="12" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="154" spans="1:1">
@@ -5414,12 +4838,12 @@
     </row>
     <row r="155" spans="1:1">
       <c r="A155" s="12" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -5429,541 +4853,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6271AA-88DA-40D4-8E32-E352C2CBA2B2}">
-  <dimension ref="A1:A192"/>
-  <sheetViews>
-    <sheetView topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="H94" sqref="H94"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="31.8">
-      <c r="A3" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="12"/>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="12" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="12"/>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="17" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="31.8">
-      <c r="A18" s="11" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="18.600000000000001">
-      <c r="A20" s="13" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="18.600000000000001">
-      <c r="A22" s="13" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="18.600000000000001">
-      <c r="A26" s="13" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="18.600000000000001">
-      <c r="A30" s="13" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="18" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" ht="18.600000000000001">
-      <c r="A38" s="13" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="12"/>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="16" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="12"/>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="16" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="15" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="15" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" ht="31.8">
-      <c r="A53" s="11" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="10" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="12"/>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" s="17" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" s="12" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" s="12"/>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="17" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" s="12" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" ht="31.8">
-      <c r="A72" s="11" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" s="12"/>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" s="12" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" ht="31.8">
-      <c r="A83" s="11" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" s="12"/>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" s="12" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" s="12"/>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" s="12" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" s="12"/>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" s="12" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" s="12"/>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" s="12" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1">
-      <c r="A93" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1">
-      <c r="A98" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1">
-      <c r="A100" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" ht="31.8">
-      <c r="A104" s="11" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" ht="18.600000000000001">
-      <c r="A106" s="13" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1">
-      <c r="A108" s="15" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" ht="18.600000000000001">
-      <c r="A110" s="13" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" ht="18.600000000000001">
-      <c r="A112" s="13" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1">
-      <c r="A114" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1">
-      <c r="A116" s="15" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" ht="18.600000000000001">
-      <c r="A118" s="13" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1">
-      <c r="A120" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1">
-      <c r="A122" s="15" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1">
-      <c r="A123" s="15" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" ht="18.600000000000001">
-      <c r="A125" s="13" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1">
-      <c r="A127" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1">
-      <c r="A128" s="12"/>
-    </row>
-    <row r="129" spans="1:1">
-      <c r="A129" s="16" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1">
-      <c r="A130" s="12"/>
-    </row>
-    <row r="131" spans="1:1">
-      <c r="A131" s="16" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1">
-      <c r="A133" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" ht="18.600000000000001">
-      <c r="A135" s="13" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" ht="16.2">
-      <c r="A137" s="19" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1">
-      <c r="A139" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" ht="16.2">
-      <c r="A141" s="19" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1">
-      <c r="A143" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" ht="16.2">
-      <c r="A145" s="19" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1">
-      <c r="A147" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" ht="31.8">
-      <c r="A151" s="11" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1">
-      <c r="A153" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1">
-      <c r="A154" s="12"/>
-    </row>
-    <row r="155" spans="1:1">
-      <c r="A155" s="12" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1">
-      <c r="A156" s="12"/>
-    </row>
-    <row r="157" spans="1:1">
-      <c r="A157" s="12" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1">
-      <c r="A158" s="12"/>
-    </row>
-    <row r="159" spans="1:1">
-      <c r="A159" s="12" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1">
-      <c r="A161" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" ht="31.8">
-      <c r="A165" s="11" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1">
-      <c r="A166" s="12"/>
-    </row>
-    <row r="167" spans="1:1">
-      <c r="A167" s="12" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1">
-      <c r="A168" s="12" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="169" spans="1:1">
-      <c r="A169" s="12"/>
-    </row>
-    <row r="170" spans="1:1">
-      <c r="A170" s="12" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1">
-      <c r="A171" s="12" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1" ht="31.8">
-      <c r="A175" s="11" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1">
-      <c r="A177" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1">
-      <c r="A178" s="12"/>
-    </row>
-    <row r="179" spans="1:1">
-      <c r="A179" s="17" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="180" spans="1:1">
-      <c r="A180" s="12"/>
-    </row>
-    <row r="181" spans="1:1">
-      <c r="A181" s="12" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="183" spans="1:1">
-      <c r="A183" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1">
-      <c r="A187" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="188" spans="1:1">
-      <c r="A188" s="12"/>
-    </row>
-    <row r="189" spans="1:1">
-      <c r="A189" s="12" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="190" spans="1:1">
-      <c r="A190" s="17" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="192" spans="1:1">
-      <c r="A192" t="s">
-        <v>500</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="18"/>
-  <hyperlinks>
-    <hyperlink ref="A34" r:id="rId1" display="https://localhost:19006/" xr:uid="{5383E6DA-55DF-463C-826C-6432F9301AB9}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>